<commit_message>
Added next day gain data to sheet and provided statistical data relative to each category
</commit_message>
<xml_diff>
--- a/Resources/SPY_Data.xlsx
+++ b/Resources/SPY_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanbruno/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanbruno/Desktop/statistical_stock_data/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17A864EB-82B5-414D-98CF-F7B69022CE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0483BBD1-95F7-A04A-920E-37F257FBAE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{359EF992-775A-204E-B5E7-1C3E78EC8A5F}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{359EF992-775A-204E-B5E7-1C3E78EC8A5F}"/>
   </bookViews>
   <sheets>
     <sheet name="SPY-2" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'SPY-2'!$A$1:$G$254</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -161,7 +161,7 @@
     <tableColumn id="6" xr3:uid="{C9038F07-9E37-F64D-AC41-CED6199C7D29}" uniqueName="6" name="Adj Close" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{B63000D8-F2BC-CB4C-A2CF-F9F811ECA8AA}" uniqueName="7" name="Volume" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{22CF37A6-0C5C-7B49-98EB-F7D38C2B2037}" uniqueName="8" name="Gain Next Day" queryTableFieldId="8" dataDxfId="0">
-      <calculatedColumnFormula>SPY_2[[#This Row],[Close]]-C1</calculatedColumnFormula>
+      <calculatedColumnFormula>(B3-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:H254"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,9 +526,9 @@
       <c r="G2">
         <v>146670500</v>
       </c>
-      <c r="H2" t="e">
-        <f>SPY_2[[#This Row],[Close]]-C1</f>
-        <v>#VALUE!</v>
+      <c r="H2">
+        <f>(B3-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.52834438016497787</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -554,8 +554,8 @@
         <v>152701600</v>
       </c>
       <c r="H3">
-        <f>SPY_2[[#This Row],[Close]]-C2</f>
-        <v>-11.520019999999988</v>
+        <f>(B4-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.3750160916637932</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -581,8 +581,8 @@
         <v>105348800</v>
       </c>
       <c r="H4">
-        <f>SPY_2[[#This Row],[Close]]-C3</f>
-        <v>4</v>
+        <f>(B5-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>6.1609940964436297E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -608,8 +608,8 @@
         <v>79595300</v>
       </c>
       <c r="H5">
-        <f>SPY_2[[#This Row],[Close]]-C4</f>
-        <v>-4.3800039999999854</v>
+        <f>(B6-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.19402907397355601</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -635,8 +635,8 @@
         <v>119940200</v>
       </c>
       <c r="H6">
-        <f>SPY_2[[#This Row],[Close]]-C5</f>
-        <v>-8.6499939999999924</v>
+        <f>(B7-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-5.2438779608546218E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -662,8 +662,8 @@
         <v>183433000</v>
       </c>
       <c r="H7">
-        <f>SPY_2[[#This Row],[Close]]-C6</f>
-        <v>-10.129975000000002</v>
+        <f>(B8-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.99813615084248708</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -689,8 +689,8 @@
         <v>152039600</v>
       </c>
       <c r="H8">
-        <f>SPY_2[[#This Row],[Close]]-C7</f>
-        <v>-0.36999500000001717</v>
+        <f>(B9-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.26848760174534109</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -716,8 +716,8 @@
         <v>123149200</v>
       </c>
       <c r="H9">
-        <f>SPY_2[[#This Row],[Close]]-C8</f>
-        <v>-3.0400089999999977</v>
+        <f>(B10-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.0819461880908836</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -743,8 +743,8 @@
         <v>113633600</v>
       </c>
       <c r="H10">
-        <f>SPY_2[[#This Row],[Close]]-C9</f>
-        <v>-0.5099800000000414</v>
+        <f>(B11-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.65087401280739421</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -770,8 +770,8 @@
         <v>109899400</v>
       </c>
       <c r="H11">
-        <f>SPY_2[[#This Row],[Close]]-C10</f>
-        <v>-0.33001699999999801</v>
+        <f>(B12-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.68022590698427576</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -797,8 +797,8 @@
         <v>86245000</v>
       </c>
       <c r="H12">
-        <f>SPY_2[[#This Row],[Close]]-C11</f>
-        <v>2.1300049999999828</v>
+        <f>(B13-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.37099890826874415</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -824,8 +824,8 @@
         <v>64653600</v>
       </c>
       <c r="H13">
-        <f>SPY_2[[#This Row],[Close]]-C12</f>
-        <v>-1.5899959999999851</v>
+        <f>(B14-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>6.8514693541669655E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -851,8 +851,8 @@
         <v>73427200</v>
       </c>
       <c r="H14">
-        <f>SPY_2[[#This Row],[Close]]-C13</f>
-        <v>2.2000130000000127</v>
+        <f>(B15-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.16649504133098533</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -878,8 +878,8 @@
         <v>73722500</v>
       </c>
       <c r="H15">
-        <f>SPY_2[[#This Row],[Close]]-C14</f>
-        <v>-0.77999799999997776</v>
+        <f>(B16-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.34856532698275533</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -905,8 +905,8 @@
         <v>97959300</v>
       </c>
       <c r="H16">
-        <f>SPY_2[[#This Row],[Close]]-C15</f>
-        <v>-0.5699769999999944</v>
+        <f>(B17-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.69979331672473954</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -932,8 +932,8 @@
         <v>115349100</v>
       </c>
       <c r="H17">
-        <f>SPY_2[[#This Row],[Close]]-C16</f>
-        <v>-6.6399840000000268</v>
+        <f>(B18-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.40870694672582081</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -959,8 +959,8 @@
         <v>113624500</v>
       </c>
       <c r="H18">
-        <f>SPY_2[[#This Row],[Close]]-C17</f>
-        <v>-7.2399900000000343</v>
+        <f>(B19-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.14121084124134545</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -986,8 +986,8 @@
         <v>73778600</v>
       </c>
       <c r="H19">
-        <f>SPY_2[[#This Row],[Close]]-C18</f>
-        <v>1.0199890000000096</v>
+        <f>(B20-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.17320665501623486</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1013,8 +1013,8 @@
         <v>90686600</v>
       </c>
       <c r="H20">
-        <f>SPY_2[[#This Row],[Close]]-C19</f>
-        <v>-4.5700069999999755</v>
+        <f>(B21-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.38510911424903727</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1040,8 +1040,8 @@
         <v>97588600</v>
       </c>
       <c r="H21">
-        <f>SPY_2[[#This Row],[Close]]-C20</f>
-        <v>-5.9400019999999927</v>
+        <f>(B22-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.39739317808455532</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1067,8 +1067,8 @@
         <v>116128600</v>
       </c>
       <c r="H22">
-        <f>SPY_2[[#This Row],[Close]]-C21</f>
-        <v>-3.0499879999999848</v>
+        <f>(B23-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.31562252043246264</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1094,8 +1094,8 @@
         <v>114409100</v>
       </c>
       <c r="H23">
-        <f>SPY_2[[#This Row],[Close]]-C22</f>
-        <v>5.4300230000000056</v>
+        <f>(B24-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.39901433307450412</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1121,8 +1121,8 @@
         <v>108107600</v>
       </c>
       <c r="H24">
-        <f>SPY_2[[#This Row],[Close]]-C23</f>
-        <v>-0.63000500000003967</v>
+        <f>(B25-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.34362170989848129</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1148,8 +1148,8 @@
         <v>76262200</v>
       </c>
       <c r="H25">
-        <f>SPY_2[[#This Row],[Close]]-C24</f>
-        <v>-2.0199890000000096</v>
+        <f>(B26-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.15453220758529929</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1175,8 +1175,8 @@
         <v>112734200</v>
       </c>
       <c r="H26">
-        <f>SPY_2[[#This Row],[Close]]-C25</f>
-        <v>0.87997500000000173</v>
+        <f>(B27-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.52229381270612152</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1202,8 +1202,8 @@
         <v>99682900</v>
       </c>
       <c r="H27">
-        <f>SPY_2[[#This Row],[Close]]-C26</f>
-        <v>2.6099849999999947</v>
+        <f>(B28-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.7114166163382093</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1229,8 +1229,8 @@
         <v>91684800</v>
       </c>
       <c r="H28">
-        <f>SPY_2[[#This Row],[Close]]-C27</f>
-        <v>5.6899720000000116</v>
+        <f>(B29-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.14764618125477391</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1256,8 +1256,8 @@
         <v>62021000</v>
       </c>
       <c r="H29">
-        <f>SPY_2[[#This Row],[Close]]-C28</f>
-        <v>-0.82000699999997551</v>
+        <f>(B30-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-4.4320152224966047E-2</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1283,8 +1283,8 @@
         <v>55836300</v>
       </c>
       <c r="H30">
-        <f>SPY_2[[#This Row],[Close]]-C29</f>
-        <v>-0.64999399999999241</v>
+        <f>(B31-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.32956959423075416</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1310,8 +1310,8 @@
         <v>57863100</v>
       </c>
       <c r="H31">
-        <f>SPY_2[[#This Row],[Close]]-C30</f>
-        <v>1.5599980000000073</v>
+        <f>(B32-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-3.1815823827412333E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1337,8 +1337,8 @@
         <v>61104600</v>
       </c>
       <c r="H32">
-        <f>SPY_2[[#This Row],[Close]]-C31</f>
-        <v>2.9100029999999606</v>
+        <f>(B33-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.15552844918535441</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1364,8 +1364,8 @@
         <v>56704900</v>
       </c>
       <c r="H33">
-        <f>SPY_2[[#This Row],[Close]]-C32</f>
-        <v>-2.9997999999977765E-2</v>
+        <f>(B34-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-2.6726264695143907E-2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1391,8 +1391,8 @@
         <v>56551000</v>
       </c>
       <c r="H34">
-        <f>SPY_2[[#This Row],[Close]]-C33</f>
-        <v>0.92999199999997018</v>
+        <f>(B35-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-7.2659015380184553E-3</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1418,8 +1418,8 @@
         <v>61659900</v>
       </c>
       <c r="H35">
-        <f>SPY_2[[#This Row],[Close]]-C34</f>
-        <v>-2.0799869999999601</v>
+        <f>(B36-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.5565628711173698</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1445,8 +1445,8 @@
         <v>60229800</v>
       </c>
       <c r="H36">
-        <f>SPY_2[[#This Row],[Close]]-C35</f>
-        <v>1.9100040000000149</v>
+        <f>(B37-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.33183567379031104</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1472,8 +1472,8 @@
         <v>82037300</v>
       </c>
       <c r="H37">
-        <f>SPY_2[[#This Row],[Close]]-C36</f>
-        <v>1.1000060000000076</v>
+        <f>(B38-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.23965872023058235</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1499,8 +1499,8 @@
         <v>78498500</v>
       </c>
       <c r="H38">
-        <f>SPY_2[[#This Row],[Close]]-C37</f>
-        <v>-2.7000130000000127</v>
+        <f>(B39-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.31309145448766124</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1526,8 +1526,8 @@
         <v>81851800</v>
       </c>
       <c r="H39">
-        <f>SPY_2[[#This Row],[Close]]-C38</f>
-        <v>-4.5699769999999944</v>
+        <f>(B40-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.16012882528646269</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1553,8 +1553,8 @@
         <v>66793000</v>
       </c>
       <c r="H40">
-        <f>SPY_2[[#This Row],[Close]]-C39</f>
-        <v>0.98001099999999042</v>
+        <f>(B41-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-4.3260027632794545E-2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1580,8 +1580,8 @@
         <v>97582800</v>
       </c>
       <c r="H41">
-        <f>SPY_2[[#This Row],[Close]]-C40</f>
-        <v>-4.0200199999999882</v>
+        <f>(B42-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.14553715186870114</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1607,8 +1607,8 @@
         <v>73209200</v>
       </c>
       <c r="H42">
-        <f>SPY_2[[#This Row],[Close]]-C41</f>
-        <v>-4.0008999999997741E-2</v>
+        <f>(B43-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.16797332072691543</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1634,8 +1634,8 @@
         <v>52182400</v>
       </c>
       <c r="H43">
-        <f>SPY_2[[#This Row],[Close]]-C42</f>
-        <v>-0.64001500000000533</v>
+        <f>(B44-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>7.6628435979573098E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1661,8 +1661,8 @@
         <v>51303100</v>
       </c>
       <c r="H44">
-        <f>SPY_2[[#This Row],[Close]]-C43</f>
-        <v>-0.70001200000001518</v>
+        <f>(B45-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>6.9459907942275245E-2</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1688,8 +1688,8 @@
         <v>51238900</v>
       </c>
       <c r="H45">
-        <f>SPY_2[[#This Row],[Close]]-C44</f>
-        <v>-0.74002100000001292</v>
+        <f>(B46-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.69957188355876765</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1715,8 +1715,8 @@
         <v>78544300</v>
       </c>
       <c r="H46">
-        <f>SPY_2[[#This Row],[Close]]-C45</f>
-        <v>1.0499879999999848</v>
+        <f>(B47-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.57848712364180521</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1742,8 +1742,8 @@
         <v>85527000</v>
       </c>
       <c r="H47">
-        <f>SPY_2[[#This Row],[Close]]-C46</f>
-        <v>-3.4200130000000399</v>
+        <f>(B48-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.51042536814068629</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1769,8 +1769,8 @@
         <v>68128300</v>
       </c>
       <c r="H48">
-        <f>SPY_2[[#This Row],[Close]]-C47</f>
-        <v>-0.33999699999998256</v>
+        <f>(B49-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.50932686247747871</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1796,8 +1796,8 @@
         <v>101591200</v>
       </c>
       <c r="H49">
-        <f>SPY_2[[#This Row],[Close]]-C48</f>
-        <v>-4.2200009999999679</v>
+        <f>(B50-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.42346615205554911</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -1823,8 +1823,8 @@
         <v>60162200</v>
       </c>
       <c r="H50">
-        <f>SPY_2[[#This Row],[Close]]-C49</f>
-        <v>-0.85000600000000759</v>
+        <f>(B51-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.9239206253762336E-2</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -1850,8 +1850,8 @@
         <v>74321400</v>
       </c>
       <c r="H51">
-        <f>SPY_2[[#This Row],[Close]]-C50</f>
-        <v>1.4400019999999927</v>
+        <f>(B52-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.19567327327246065</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1877,8 +1877,8 @@
         <v>67733800</v>
       </c>
       <c r="H52">
-        <f>SPY_2[[#This Row],[Close]]-C51</f>
-        <v>2.9100040000000149</v>
+        <f>(B53-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>9.0022980313923015E-2</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1904,8 +1904,8 @@
         <v>81852400</v>
       </c>
       <c r="H53">
-        <f>SPY_2[[#This Row],[Close]]-C52</f>
-        <v>-4.8800049999999828</v>
+        <f>(B54-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.1580600030719206</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -1931,8 +1931,8 @@
         <v>116888000</v>
       </c>
       <c r="H54">
-        <f>SPY_2[[#This Row],[Close]]-C53</f>
-        <v>-8.5299989999999752</v>
+        <f>(B55-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.71943701618728262</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -1958,8 +1958,8 @@
         <v>134811000</v>
       </c>
       <c r="H55">
-        <f>SPY_2[[#This Row],[Close]]-C54</f>
-        <v>-9.8599849999999947</v>
+        <f>(B56-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.4094627620486545</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -1985,8 +1985,8 @@
         <v>106394000</v>
       </c>
       <c r="H56">
-        <f>SPY_2[[#This Row],[Close]]-C55</f>
-        <v>-2.3099970000000098</v>
+        <f>(B57-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.71414448843264888</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2012,8 +2012,8 @@
         <v>82201600</v>
       </c>
       <c r="H57">
-        <f>SPY_2[[#This Row],[Close]]-C56</f>
-        <v>4.2299810000000093</v>
+        <f>(B58-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.28565270467493953</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2039,8 +2039,8 @@
         <v>65129200</v>
       </c>
       <c r="H58">
-        <f>SPY_2[[#This Row],[Close]]-C57</f>
-        <v>-1.9700009999999679</v>
+        <f>(B59-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>6.7385205865505365E-2</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2066,8 +2066,8 @@
         <v>59810200</v>
       </c>
       <c r="H59">
-        <f>SPY_2[[#This Row],[Close]]-C58</f>
-        <v>-4.4500130000000127</v>
+        <f>(B60-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.2186213952584313</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2093,8 +2093,8 @@
         <v>106467100</v>
       </c>
       <c r="H60">
-        <f>SPY_2[[#This Row],[Close]]-C59</f>
-        <v>-5.2000130000000127</v>
+        <f>(B61-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.22878913360228795</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2120,8 +2120,8 @@
         <v>78022200</v>
       </c>
       <c r="H61">
-        <f>SPY_2[[#This Row],[Close]]-C60</f>
-        <v>4.2300109999999904</v>
+        <f>(B62-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.382873243071849</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2147,8 +2147,8 @@
         <v>76578700</v>
       </c>
       <c r="H62">
-        <f>SPY_2[[#This Row],[Close]]-C61</f>
-        <v>-1.6900029999999902</v>
+        <f>(B63-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.57839542787682163</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2174,8 +2174,8 @@
         <v>51376700</v>
       </c>
       <c r="H63">
-        <f>SPY_2[[#This Row],[Close]]-C62</f>
-        <v>0.97000099999996792</v>
+        <f>(B64-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.27673115061311265</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2201,8 +2201,8 @@
         <v>57451400</v>
       </c>
       <c r="H64">
-        <f>SPY_2[[#This Row],[Close]]-C63</f>
-        <v>-2.080016999999998</v>
+        <f>(B65-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.15063241561382967</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2228,8 +2228,8 @@
         <v>43088600</v>
       </c>
       <c r="H65">
-        <f>SPY_2[[#This Row],[Close]]-C64</f>
-        <v>-1.6399840000000268</v>
+        <f>(B66-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.2624874082196027</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2255,8 +2255,8 @@
         <v>56707700</v>
       </c>
       <c r="H66">
-        <f>SPY_2[[#This Row],[Close]]-C65</f>
-        <v>-0.31997599999999693</v>
+        <f>(B67-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.40067541890797287</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2282,8 +2282,8 @@
         <v>58520200</v>
       </c>
       <c r="H67">
-        <f>SPY_2[[#This Row],[Close]]-C66</f>
-        <v>-0.67999200000002702</v>
+        <f>(B68-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.60232309917886362</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2309,8 +2309,8 @@
         <v>54216600</v>
       </c>
       <c r="H68">
-        <f>SPY_2[[#This Row],[Close]]-C67</f>
-        <v>-1.5799870000000169</v>
+        <f>(B69-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.16679342776869649</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -2336,8 +2336,8 @@
         <v>49097100</v>
       </c>
       <c r="H69">
-        <f>SPY_2[[#This Row],[Close]]-C68</f>
-        <v>-2.3900140000000079</v>
+        <f>(B70-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.590008107130365</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2363,8 +2363,8 @@
         <v>58138800</v>
       </c>
       <c r="H70">
-        <f>SPY_2[[#This Row],[Close]]-C69</f>
-        <v>-2.4600219999999808</v>
+        <f>(B71-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.47281587793054347</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2390,8 +2390,8 @@
         <v>55938800</v>
       </c>
       <c r="H71">
-        <f>SPY_2[[#This Row],[Close]]-C70</f>
-        <v>2.6100160000000301</v>
+        <f>(B72-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-2.3686701036209875E-3</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2417,8 +2417,8 @@
         <v>51555000</v>
       </c>
       <c r="H72">
-        <f>SPY_2[[#This Row],[Close]]-C71</f>
-        <v>-0.73001099999999042</v>
+        <f>(B73-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.2179073392647517</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2444,8 +2444,8 @@
         <v>47134300</v>
       </c>
       <c r="H73">
-        <f>SPY_2[[#This Row],[Close]]-C72</f>
-        <v>-0.5</v>
+        <f>(B74-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.21312730939929014</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -2471,8 +2471,8 @@
         <v>48436300</v>
       </c>
       <c r="H74">
-        <f>SPY_2[[#This Row],[Close]]-C73</f>
-        <v>-1.5599970000000098</v>
+        <f>(B75-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.31068350969785852</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -2498,8 +2498,8 @@
         <v>51020100</v>
       </c>
       <c r="H75">
-        <f>SPY_2[[#This Row],[Close]]-C74</f>
-        <v>0.34997499999997217</v>
+        <f>(B76-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.13928543256600065</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2525,8 +2525,8 @@
         <v>45570800</v>
       </c>
       <c r="H76">
-        <f>SPY_2[[#This Row],[Close]]-C75</f>
-        <v>-0.32000699999997551</v>
+        <f>(B77-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>2.8280031242633404E-2</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2552,8 +2552,8 @@
         <v>42358500</v>
       </c>
       <c r="H77">
-        <f>SPY_2[[#This Row],[Close]]-C76</f>
-        <v>0.83001699999999801</v>
+        <f>(B78-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>3.7624746328713245E-2</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2579,8 +2579,8 @@
         <v>51508500</v>
       </c>
       <c r="H78">
-        <f>SPY_2[[#This Row],[Close]]-C77</f>
-        <v>-0.88998400000002675</v>
+        <f>(B79-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>3.5335939529080068E-2</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2606,8 +2606,8 @@
         <v>80386100</v>
       </c>
       <c r="H79">
-        <f>SPY_2[[#This Row],[Close]]-C78</f>
-        <v>-3.3500060000000076</v>
+        <f>(B80-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.10423160210247374</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2633,8 +2633,8 @@
         <v>90949700</v>
       </c>
       <c r="H80">
-        <f>SPY_2[[#This Row],[Close]]-C79</f>
-        <v>-2.8999939999999924</v>
+        <f>(B81-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.156481500683751</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2660,8 +2660,8 @@
         <v>118676300</v>
       </c>
       <c r="H81">
-        <f>SPY_2[[#This Row],[Close]]-C80</f>
-        <v>-8.0999760000000265</v>
+        <f>(B82-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.45309335320010263</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2687,8 +2687,8 @@
         <v>72822000</v>
       </c>
       <c r="H82">
-        <f>SPY_2[[#This Row],[Close]]-C81</f>
-        <v>3.0299979999999778</v>
+        <f>(B83-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-2.3710973615101664E-3</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2714,8 +2714,8 @@
         <v>57700300</v>
       </c>
       <c r="H83">
-        <f>SPY_2[[#This Row],[Close]]-C82</f>
-        <v>2.0499869999999873</v>
+        <f>(B84-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.8911631215698679E-2</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2741,8 +2741,8 @@
         <v>49445400</v>
       </c>
       <c r="H84">
-        <f>SPY_2[[#This Row],[Close]]-C83</f>
-        <v>-1.3999939999999924</v>
+        <f>(B85-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.54188569983124835</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -2768,8 +2768,8 @@
         <v>45110300</v>
       </c>
       <c r="H85">
-        <f>SPY_2[[#This Row],[Close]]-C84</f>
-        <v>1.0500180000000228</v>
+        <f>(B86-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.18818818835772605</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -2795,8 +2795,8 @@
         <v>58129500</v>
       </c>
       <c r="H86">
-        <f>SPY_2[[#This Row],[Close]]-C85</f>
-        <v>1.0599970000000098</v>
+        <f>(B87-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.13127400194348204</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2822,8 +2822,8 @@
         <v>53159600</v>
       </c>
       <c r="H87">
-        <f>SPY_2[[#This Row],[Close]]-C86</f>
-        <v>0.38000500000003967</v>
+        <f>(B88-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>9.5914099010648013E-2</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2849,8 +2849,8 @@
         <v>35970500</v>
       </c>
       <c r="H88">
-        <f>SPY_2[[#This Row],[Close]]-C87</f>
-        <v>5.0018000000022766E-2</v>
+        <f>(B89-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.11457119154815758</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -2876,8 +2876,8 @@
         <v>64827900</v>
       </c>
       <c r="H89">
-        <f>SPY_2[[#This Row],[Close]]-C88</f>
-        <v>-0.5</v>
+        <f>(B90-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.18922510951373922</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -2903,8 +2903,8 @@
         <v>53441000</v>
       </c>
       <c r="H90">
-        <f>SPY_2[[#This Row],[Close]]-C89</f>
-        <v>1.6499940000000493</v>
+        <f>(B91-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.28808866021563667</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -2930,8 +2930,8 @@
         <v>57697700</v>
       </c>
       <c r="H91">
-        <f>SPY_2[[#This Row],[Close]]-C90</f>
-        <v>3.1199950000000172</v>
+        <f>(B92-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.3833348672327075E-2</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -2957,8 +2957,8 @@
         <v>68710400</v>
       </c>
       <c r="H92">
-        <f>SPY_2[[#This Row],[Close]]-C91</f>
-        <v>-1.1700129999999831</v>
+        <f>(B93-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.1686210269104618</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -2984,8 +2984,8 @@
         <v>63549500</v>
       </c>
       <c r="H93">
-        <f>SPY_2[[#This Row],[Close]]-C92</f>
-        <v>0.44998099999997976</v>
+        <f>(B94-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.3073682543072249</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -3011,8 +3011,8 @@
         <v>97595200</v>
       </c>
       <c r="H94">
-        <f>SPY_2[[#This Row],[Close]]-C93</f>
-        <v>-3.8399970000000394</v>
+        <f>(B95-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.37361597313420486</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -3038,8 +3038,8 @@
         <v>76238600</v>
       </c>
       <c r="H95">
-        <f>SPY_2[[#This Row],[Close]]-C94</f>
-        <v>3.7899780000000192</v>
+        <f>(B96-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-2.0664034320588921E-2</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -3065,8 +3065,8 @@
         <v>52889600</v>
       </c>
       <c r="H96">
-        <f>SPY_2[[#This Row],[Close]]-C95</f>
-        <v>1.2399910000000318</v>
+        <f>(B97-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.19218381646012986</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -3092,8 +3092,8 @@
         <v>52911300</v>
       </c>
       <c r="H97">
-        <f>SPY_2[[#This Row],[Close]]-C96</f>
-        <v>-1.7600100000000225</v>
+        <f>(B98-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.41552790849677995</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -3119,8 +3119,8 @@
         <v>64130400</v>
       </c>
       <c r="H98">
-        <f>SPY_2[[#This Row],[Close]]-C97</f>
-        <v>-1.6000060000000076</v>
+        <f>(B99-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.32779938400419689</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3146,8 +3146,8 @@
         <v>55126400</v>
       </c>
       <c r="H99">
-        <f>SPY_2[[#This Row],[Close]]-C98</f>
-        <v>-3.1700129999999831</v>
+        <f>(B100-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.28982403680276536</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -3173,8 +3173,8 @@
         <v>75874700</v>
       </c>
       <c r="H100">
-        <f>SPY_2[[#This Row],[Close]]-C99</f>
-        <v>-4.1900029999999902</v>
+        <f>(B101-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.1939523456572743</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -3200,8 +3200,8 @@
         <v>147987000</v>
       </c>
       <c r="H101">
-        <f>SPY_2[[#This Row],[Close]]-C100</f>
-        <v>-11.089996999999983</v>
+        <f>(B102-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.16706873387046434</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -3227,8 +3227,8 @@
         <v>99608200</v>
       </c>
       <c r="H102">
-        <f>SPY_2[[#This Row],[Close]]-C101</f>
-        <v>-0.35000600000000759</v>
+        <f>(B103-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.29694195841386739</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -3254,8 +3254,8 @@
         <v>64724400</v>
       </c>
       <c r="H103">
-        <f>SPY_2[[#This Row],[Close]]-C102</f>
-        <v>2.1299750000000017</v>
+        <f>(B104-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>4.3723853468382257E-2</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -3281,8 +3281,8 @@
         <v>47878500</v>
       </c>
       <c r="H104">
-        <f>SPY_2[[#This Row],[Close]]-C103</f>
-        <v>0.75997899999998708</v>
+        <f>(B105-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.47306251838874613</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -3308,8 +3308,8 @@
         <v>63766600</v>
       </c>
       <c r="H105">
-        <f>SPY_2[[#This Row],[Close]]-C104</f>
-        <v>4.2200009999999679</v>
+        <f>(B106-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.14320225420192306</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -3335,8 +3335,8 @@
         <v>43719200</v>
       </c>
       <c r="H106">
-        <f>SPY_2[[#This Row],[Close]]-C105</f>
-        <v>0.72000100000002476</v>
+        <f>(B107-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.251685870864233</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -3362,8 +3362,8 @@
         <v>67397100</v>
       </c>
       <c r="H107">
-        <f>SPY_2[[#This Row],[Close]]-C106</f>
-        <v>-2.0199889999999527</v>
+        <f>(B108-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.1526122377027353</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -3389,8 +3389,8 @@
         <v>52472400</v>
       </c>
       <c r="H108">
-        <f>SPY_2[[#This Row],[Close]]-C107</f>
-        <v>-1.1100149999999758</v>
+        <f>(B109-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.22560445487513109</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -3416,8 +3416,8 @@
         <v>47435300</v>
       </c>
       <c r="H109">
-        <f>SPY_2[[#This Row],[Close]]-C108</f>
-        <v>0.35000600000000759</v>
+        <f>(B110-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.62180643079731379</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -3443,8 +3443,8 @@
         <v>68890600</v>
       </c>
       <c r="H110">
-        <f>SPY_2[[#This Row],[Close]]-C109</f>
-        <v>-3.2899779999999623</v>
+        <f>(B111-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.41731909381041554</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -3470,8 +3470,8 @@
         <v>58783300</v>
       </c>
       <c r="H111">
-        <f>SPY_2[[#This Row],[Close]]-C110</f>
-        <v>-2.4700020000000222</v>
+        <f>(B112-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.19424712808105596</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -3497,8 +3497,8 @@
         <v>58053900</v>
       </c>
       <c r="H112">
-        <f>SPY_2[[#This Row],[Close]]-C111</f>
-        <v>0.22000099999996792</v>
+        <f>(B113-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.31055083727373173</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -3524,8 +3524,8 @@
         <v>46732200</v>
       </c>
       <c r="H113">
-        <f>SPY_2[[#This Row],[Close]]-C112</f>
-        <v>-2.2999879999999848</v>
+        <f>(B114-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.28247072051762157</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -3551,8 +3551,8 @@
         <v>38969700</v>
       </c>
       <c r="H114">
-        <f>SPY_2[[#This Row],[Close]]-C113</f>
-        <v>0.64001500000000533</v>
+        <f>(B115-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>7.6963960590272773E-2</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -3578,8 +3578,8 @@
         <v>46864100</v>
       </c>
       <c r="H115">
-        <f>SPY_2[[#This Row],[Close]]-C114</f>
-        <v>0.63998399999996991</v>
+        <f>(B116-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-6.7795883924911477E-3</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -3605,8 +3605,8 @@
         <v>41222600</v>
       </c>
       <c r="H116">
-        <f>SPY_2[[#This Row],[Close]]-C115</f>
-        <v>-0.80999700000000985</v>
+        <f>(B117-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.10856082929725881</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -3632,8 +3632,8 @@
         <v>43339300</v>
       </c>
       <c r="H117">
-        <f>SPY_2[[#This Row],[Close]]-C116</f>
-        <v>-0.11999499999996033</v>
+        <f>(B118-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.25752553041175069</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -3659,8 +3659,8 @@
         <v>44034300</v>
       </c>
       <c r="H118">
-        <f>SPY_2[[#This Row],[Close]]-C117</f>
-        <v>0.33999699999998256</v>
+        <f>(B119-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-3.6054802010119E-2</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -3686,8 +3686,8 @@
         <v>38909400</v>
       </c>
       <c r="H119">
-        <f>SPY_2[[#This Row],[Close]]-C118</f>
-        <v>1.2299800000000118</v>
+        <f>(B120-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.10784098676195512</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -3713,8 +3713,8 @@
         <v>39388300</v>
       </c>
       <c r="H120">
-        <f>SPY_2[[#This Row],[Close]]-C119</f>
-        <v>0.66000299999996059</v>
+        <f>(B121-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.31171823633760248</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -3740,8 +3740,8 @@
         <v>73740000</v>
       </c>
       <c r="H121">
-        <f>SPY_2[[#This Row],[Close]]-C120</f>
-        <v>1.0299990000000321</v>
+        <f>(B122-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.61078170657812159</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -3767,8 +3767,8 @@
         <v>92673900</v>
       </c>
       <c r="H122">
-        <f>SPY_2[[#This Row],[Close]]-C121</f>
-        <v>-3.0699759999999969</v>
+        <f>(B123-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.24322538017064033</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -3794,8 +3794,8 @@
         <v>89351900</v>
       </c>
       <c r="H123">
-        <f>SPY_2[[#This Row],[Close]]-C122</f>
-        <v>-5.7799979999999778</v>
+        <f>(B124-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.66259940033288689</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -3821,8 +3821,8 @@
         <v>92812200</v>
       </c>
       <c r="H124">
-        <f>SPY_2[[#This Row],[Close]]-C123</f>
-        <v>-4.7700199999999882</v>
+        <f>(B125-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>8.4123587645735895E-2</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -3848,8 +3848,8 @@
         <v>71975900</v>
       </c>
       <c r="H125">
-        <f>SPY_2[[#This Row],[Close]]-C124</f>
-        <v>2.2199699999999893</v>
+        <f>(B126-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.40599491629810036</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
@@ -3875,8 +3875,8 @@
         <v>54973000</v>
       </c>
       <c r="H126">
-        <f>SPY_2[[#This Row],[Close]]-C125</f>
-        <v>3.5500190000000202</v>
+        <f>(B127-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.15874233871255386</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
@@ -3902,8 +3902,8 @@
         <v>38744700</v>
       </c>
       <c r="H127">
-        <f>SPY_2[[#This Row],[Close]]-C126</f>
-        <v>-0.26000999999996566</v>
+        <f>(B128-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>4.4648525471230903E-2</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
@@ -3929,8 +3929,8 @@
         <v>40529700</v>
       </c>
       <c r="H128">
-        <f>SPY_2[[#This Row],[Close]]-C127</f>
-        <v>0.36999500000001717</v>
+        <f>(B129-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-6.683277212062759E-2</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
@@ -3956,8 +3956,8 @@
         <v>57829600</v>
       </c>
       <c r="H129">
-        <f>SPY_2[[#This Row],[Close]]-C128</f>
-        <v>-3.1999809999999798</v>
+        <f>(B130-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.19270940275378801</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
@@ -3983,8 +3983,8 @@
         <v>77201900</v>
       </c>
       <c r="H130">
-        <f>SPY_2[[#This Row],[Close]]-C129</f>
-        <v>1.3900150000000053</v>
+        <f>(B131-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.15991138256524703</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -4010,8 +4010,8 @@
         <v>48357400</v>
       </c>
       <c r="H131">
-        <f>SPY_2[[#This Row],[Close]]-C130</f>
-        <v>1.580016999999998</v>
+        <f>(B132-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-2.2113968017926963E-2</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
@@ -4037,8 +4037,8 @@
         <v>59300200</v>
       </c>
       <c r="H132">
-        <f>SPY_2[[#This Row],[Close]]-C131</f>
-        <v>-1.5100089999999682</v>
+        <f>(B133-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.2214545142238219</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -4064,8 +4064,8 @@
         <v>48721400</v>
       </c>
       <c r="H133">
-        <f>SPY_2[[#This Row],[Close]]-C132</f>
-        <v>-0.69000199999999268</v>
+        <f>(B134-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.33643626391596781</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -4091,8 +4091,8 @@
         <v>42501000</v>
       </c>
       <c r="H134">
-        <f>SPY_2[[#This Row],[Close]]-C133</f>
-        <v>8.0016999999998006E-2</v>
+        <f>(B135-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.26699419551625553</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
@@ -4118,8 +4118,8 @@
         <v>47170500</v>
       </c>
       <c r="H135">
-        <f>SPY_2[[#This Row],[Close]]-C134</f>
-        <v>-0.97000099999996792</v>
+        <f>(B136-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-8.1662401919335853E-2</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -4145,8 +4145,8 @@
         <v>51671500</v>
       </c>
       <c r="H136">
-        <f>SPY_2[[#This Row],[Close]]-C135</f>
-        <v>-2.1700139999999806</v>
+        <f>(B137-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.12625171916950598</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -4172,8 +4172,8 @@
         <v>56181900</v>
       </c>
       <c r="H137">
-        <f>SPY_2[[#This Row],[Close]]-C136</f>
-        <v>-1.8999939999999924</v>
+        <f>(B138-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-4.6570712145920748E-2</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
@@ -4199,8 +4199,8 @@
         <v>57970400</v>
       </c>
       <c r="H138">
-        <f>SPY_2[[#This Row],[Close]]-C137</f>
-        <v>-2.6900019999999927</v>
+        <f>(B139-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.45881730801597026</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
@@ -4226,8 +4226,8 @@
         <v>89848000</v>
       </c>
       <c r="H139">
-        <f>SPY_2[[#This Row],[Close]]-C138</f>
-        <v>-7.1300049999999828</v>
+        <f>(B140-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.71839371983480116</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
@@ -4253,8 +4253,8 @@
         <v>83738600</v>
       </c>
       <c r="H140">
-        <f>SPY_2[[#This Row],[Close]]-C139</f>
-        <v>-4.9100029999999606</v>
+        <f>(B141-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.34484483067531646</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -4280,8 +4280,8 @@
         <v>78197100</v>
       </c>
       <c r="H141">
-        <f>SPY_2[[#This Row],[Close]]-C140</f>
-        <v>-4.75</v>
+        <f>(B142-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.10130850503859523</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
@@ -4307,8 +4307,8 @@
         <v>78792200</v>
       </c>
       <c r="H142">
-        <f>SPY_2[[#This Row],[Close]]-C141</f>
-        <v>-0.45999100000000226</v>
+        <f>(B143-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.12503304316967828</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -4334,8 +4334,8 @@
         <v>77786700</v>
       </c>
       <c r="H143">
-        <f>SPY_2[[#This Row],[Close]]-C142</f>
-        <v>-1.2399910000000318</v>
+        <f>(B144-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.50316433002854333</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
@@ -4361,8 +4361,8 @@
         <v>118425000</v>
       </c>
       <c r="H144">
-        <f>SPY_2[[#This Row],[Close]]-C143</f>
-        <v>-6.9599910000000023</v>
+        <f>(B145-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.4771157880894783</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
@@ -4388,8 +4388,8 @@
         <v>166445500</v>
       </c>
       <c r="H145">
-        <f>SPY_2[[#This Row],[Close]]-C144</f>
-        <v>-11.329986000000019</v>
+        <f>(B146-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.57367752934499128</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -4415,8 +4415,8 @@
         <v>92526100</v>
       </c>
       <c r="H146">
-        <f>SPY_2[[#This Row],[Close]]-C145</f>
-        <v>-2.9299930000000245</v>
+        <f>(B147-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.55807554184355901</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -4442,8 +4442,8 @@
         <v>102350100</v>
       </c>
       <c r="H147">
-        <f>SPY_2[[#This Row],[Close]]-C146</f>
-        <v>-5.0019000000020242E-2</v>
+        <f>(B148-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.45448797975910332</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
@@ -4469,8 +4469,8 @@
         <v>76396000</v>
       </c>
       <c r="H148">
-        <f>SPY_2[[#This Row],[Close]]-C147</f>
-        <v>3.1499940000000493</v>
+        <f>(B149-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.39261497077554935</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -4496,8 +4496,8 @@
         <v>62094800</v>
       </c>
       <c r="H149">
-        <f>SPY_2[[#This Row],[Close]]-C148</f>
-        <v>-0.98001099999999042</v>
+        <f>(B150-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.24779932645987579</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
@@ -4523,8 +4523,8 @@
         <v>61371100</v>
       </c>
       <c r="H150">
-        <f>SPY_2[[#This Row],[Close]]-C149</f>
-        <v>-2.0299979999999778</v>
+        <f>(B151-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.66645872493023761</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -4550,8 +4550,8 @@
         <v>130436300</v>
       </c>
       <c r="H151">
-        <f>SPY_2[[#This Row],[Close]]-C150</f>
-        <v>-10.32998699999996</v>
+        <f>(B152-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.33892857064711845</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -4577,8 +4577,8 @@
         <v>82329200</v>
       </c>
       <c r="H152">
-        <f>SPY_2[[#This Row],[Close]]-C151</f>
-        <v>-5.5899969999999826</v>
+        <f>(B153-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.36137114895510564</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -4604,8 +4604,8 @@
         <v>140181200</v>
       </c>
       <c r="H153">
-        <f>SPY_2[[#This Row],[Close]]-C152</f>
-        <v>-7.8999939999999924</v>
+        <f>(B154-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.42876355867210031</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -4631,8 +4631,8 @@
         <v>129240100</v>
       </c>
       <c r="H154">
-        <f>SPY_2[[#This Row],[Close]]-C153</f>
-        <v>-2.5299990000000321</v>
+        <f>(B155-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.28555407805715394</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
@@ -4658,8 +4658,8 @@
         <v>128570000</v>
       </c>
       <c r="H155">
-        <f>SPY_2[[#This Row],[Close]]-C154</f>
-        <v>-7.3899839999999699</v>
+        <f>(B156-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.37326776409336682</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
@@ -4685,8 +4685,8 @@
         <v>90682500</v>
       </c>
       <c r="H156">
-        <f>SPY_2[[#This Row],[Close]]-C155</f>
-        <v>-0.85998499999999467</v>
+        <f>(B157-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.88432624034643814</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
@@ -4712,8 +4712,8 @@
         <v>113032200</v>
       </c>
       <c r="H157">
-        <f>SPY_2[[#This Row],[Close]]-C156</f>
-        <v>-0.58999599999998509</v>
+        <f>(B158-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.80248816926863709</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -4739,8 +4739,8 @@
         <v>72437500</v>
       </c>
       <c r="H158">
-        <f>SPY_2[[#This Row],[Close]]-C157</f>
-        <v>3.5400089999999977</v>
+        <f>(B159-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.18693452617576128</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -4766,8 +4766,8 @@
         <v>74492900</v>
       </c>
       <c r="H159">
-        <f>SPY_2[[#This Row],[Close]]-C158</f>
-        <v>-3.8200080000000298</v>
+        <f>(B160-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.15986411729310676</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -4793,8 +4793,8 @@
         <v>65233300</v>
       </c>
       <c r="H160">
-        <f>SPY_2[[#This Row],[Close]]-C159</f>
-        <v>-5.2000130000000127</v>
+        <f>(B161-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.22545054993006039</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -4820,8 +4820,8 @@
         <v>71181200</v>
       </c>
       <c r="H161">
-        <f>SPY_2[[#This Row],[Close]]-C160</f>
-        <v>-6.6400150000000053</v>
+        <f>(B162-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.25137124961222901</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
@@ -4847,8 +4847,8 @@
         <v>72974000</v>
       </c>
       <c r="H162">
-        <f>SPY_2[[#This Row],[Close]]-C161</f>
-        <v>-0.92001299999998309</v>
+        <f>(B163-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.89617952634141251</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
@@ -4874,8 +4874,8 @@
         <v>70236800</v>
       </c>
       <c r="H163">
-        <f>SPY_2[[#This Row],[Close]]-C162</f>
-        <v>6.4500120000000152</v>
+        <f>(B164-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.50847457627118642</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
@@ -4901,8 +4901,8 @@
         <v>66226800</v>
       </c>
       <c r="H164">
-        <f>SPY_2[[#This Row],[Close]]-C163</f>
-        <v>3.2099910000000023</v>
+        <f>(B165-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.42613183692703799</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -4928,8 +4928,8 @@
         <v>62213200</v>
       </c>
       <c r="H165">
-        <f>SPY_2[[#This Row],[Close]]-C164</f>
-        <v>0.92999199999997018</v>
+        <f>(B166-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.3868626293662063</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
@@ -4955,8 +4955,8 @@
         <v>46996800</v>
       </c>
       <c r="H166">
-        <f>SPY_2[[#This Row],[Close]]-C165</f>
-        <v>3.0900270000000205</v>
+        <f>(B167-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.10873202194438447</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
@@ -4982,8 +4982,8 @@
         <v>49571600</v>
       </c>
       <c r="H167">
-        <f>SPY_2[[#This Row],[Close]]-C166</f>
-        <v>1.7000130000000127</v>
+        <f>(B168-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.14146791501984676</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
@@ -5009,8 +5009,8 @@
         <v>41305400</v>
       </c>
       <c r="H168">
-        <f>SPY_2[[#This Row],[Close]]-C167</f>
-        <v>0.85998499999999467</v>
+        <f>(B169-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.10141118720793001</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -5036,8 +5036,8 @@
         <v>58845100</v>
       </c>
       <c r="H169">
-        <f>SPY_2[[#This Row],[Close]]-C168</f>
-        <v>-0.70999199999999973</v>
+        <f>(B170-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.25600371045200909</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
@@ -5063,8 +5063,8 @@
         <v>45214500</v>
       </c>
       <c r="H170">
-        <f>SPY_2[[#This Row],[Close]]-C169</f>
-        <v>0.87997500000000173</v>
+        <f>(B171-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.36220481691682765</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -5090,8 +5090,8 @@
         <v>56075100</v>
       </c>
       <c r="H171">
-        <f>SPY_2[[#This Row],[Close]]-C170</f>
-        <v>5.9997000000009848E-2</v>
+        <f>(B172-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.10747017494348818</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -5117,8 +5117,8 @@
         <v>72438000</v>
       </c>
       <c r="H172">
-        <f>SPY_2[[#This Row],[Close]]-C171</f>
-        <v>-4.5499879999999848</v>
+        <f>(B173-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.33484359018882187</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
@@ -5144,8 +5144,8 @@
         <v>51437900</v>
       </c>
       <c r="H173">
-        <f>SPY_2[[#This Row],[Close]]-C172</f>
-        <v>1.1600029999999606</v>
+        <f>(B174-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.53456361550456133</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -5171,8 +5171,8 @@
         <v>70108200</v>
       </c>
       <c r="H174">
-        <f>SPY_2[[#This Row],[Close]]-C173</f>
-        <v>0.85000600000000759</v>
+        <f>(B175-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.22863102885138484</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -5198,8 +5198,8 @@
         <v>48433600</v>
       </c>
       <c r="H175">
-        <f>SPY_2[[#This Row],[Close]]-C174</f>
-        <v>0.48001099999999042</v>
+        <f>(B176-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>3.9125292687320817E-2</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -5225,8 +5225,8 @@
         <v>48908400</v>
       </c>
       <c r="H176">
-        <f>SPY_2[[#This Row],[Close]]-C175</f>
-        <v>1.1999819999999772</v>
+        <f>(B177-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.12989954704351167</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
@@ -5252,8 +5252,8 @@
         <v>52509800</v>
       </c>
       <c r="H177">
-        <f>SPY_2[[#This Row],[Close]]-C176</f>
-        <v>2.4899900000000343</v>
+        <f>(B178-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.1377138919398414</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -5279,8 +5279,8 @@
         <v>52847100</v>
       </c>
       <c r="H178">
-        <f>SPY_2[[#This Row],[Close]]-C177</f>
-        <v>1.7600100000000225</v>
+        <f>(B179-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.50759139442211654</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
@@ -5306,8 +5306,8 @@
         <v>66332200</v>
       </c>
       <c r="H179">
-        <f>SPY_2[[#This Row],[Close]]-C178</f>
-        <v>1.5299989999999752</v>
+        <f>(B180-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.24971997577470806</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -5333,8 +5333,8 @@
         <v>50405200</v>
       </c>
       <c r="H180">
-        <f>SPY_2[[#This Row],[Close]]-C179</f>
-        <v>-1.7200009999999679</v>
+        <f>(B181-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>8.3171050225390675E-2</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
@@ -5360,8 +5360,8 @@
         <v>51149100</v>
       </c>
       <c r="H181">
-        <f>SPY_2[[#This Row],[Close]]-C180</f>
-        <v>-2.8500060000000076</v>
+        <f>(B182-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.38512944087113138</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -5387,8 +5387,8 @@
         <v>69429700</v>
       </c>
       <c r="H182">
-        <f>SPY_2[[#This Row],[Close]]-C181</f>
-        <v>-5.9500119999999583</v>
+        <f>(B183-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.3429524216271097</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -5414,8 +5414,8 @@
         <v>34848500</v>
       </c>
       <c r="H183">
-        <f>SPY_2[[#This Row],[Close]]-C182</f>
-        <v>-3.6100159999999732</v>
+        <f>(B184-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.29109386808554522</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
@@ -5441,8 +5441,8 @@
         <v>53423300</v>
       </c>
       <c r="H184">
-        <f>SPY_2[[#This Row],[Close]]-C183</f>
-        <v>1.9799800000000118</v>
+        <f>(B185-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.29319794385510939</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
@@ -5468,8 +5468,8 @@
         <v>46980500</v>
       </c>
       <c r="H185">
-        <f>SPY_2[[#This Row],[Close]]-C184</f>
-        <v>-0.42999199999997018</v>
+        <f>(B186-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-5.9901804375662324E-2</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -5495,8 +5495,8 @@
         <v>48857500</v>
       </c>
       <c r="H186">
-        <f>SPY_2[[#This Row],[Close]]-C185</f>
-        <v>0.47000099999996792</v>
+        <f>(B187-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-5.9665658156459224E-2</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -5522,8 +5522,8 @@
         <v>47858300</v>
       </c>
       <c r="H187">
-        <f>SPY_2[[#This Row],[Close]]-C186</f>
-        <v>-2.3499749999999722</v>
+        <f>(B188-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.23496709632906987</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
@@ -5549,8 +5549,8 @@
         <v>50625600</v>
       </c>
       <c r="H188">
-        <f>SPY_2[[#This Row],[Close]]-C187</f>
-        <v>0.54000899999999774</v>
+        <f>(B189-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-2.5552125090852616E-2</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
@@ -5576,8 +5576,8 @@
         <v>57315600</v>
       </c>
       <c r="H189">
-        <f>SPY_2[[#This Row],[Close]]-C188</f>
-        <v>-1.1199950000000172</v>
+        <f>(B190-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.42653925995843611</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
@@ -5603,8 +5603,8 @@
         <v>72762000</v>
       </c>
       <c r="H190">
-        <f>SPY_2[[#This Row],[Close]]-C189</f>
-        <v>-3.3699950000000172</v>
+        <f>(B191-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-7.4856384019505937E-2</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
@@ -5630,8 +5630,8 @@
         <v>73206500</v>
       </c>
       <c r="H191">
-        <f>SPY_2[[#This Row],[Close]]-C190</f>
-        <v>-5.3500070000000051</v>
+        <f>(B192-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.45494435825222623</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
@@ -5657,8 +5657,8 @@
         <v>61858800</v>
       </c>
       <c r="H192">
-        <f>SPY_2[[#This Row],[Close]]-C191</f>
-        <v>0.33999599999998509</v>
+        <f>(B193-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.5124416261399061</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
@@ -5684,8 +5684,8 @@
         <v>112669600</v>
       </c>
       <c r="H193">
-        <f>SPY_2[[#This Row],[Close]]-C192</f>
-        <v>-10.600005999999951</v>
+        <f>(B194-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.1111850423531169</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
@@ -5711,8 +5711,8 @@
         <v>86268800</v>
       </c>
       <c r="H194">
-        <f>SPY_2[[#This Row],[Close]]-C193</f>
-        <v>0.70001200000001518</v>
+        <f>(B195-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.5596224637155961</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
@@ -5738,8 +5738,8 @@
         <v>148559600</v>
       </c>
       <c r="H195">
-        <f>SPY_2[[#This Row],[Close]]-C194</f>
-        <v>-11</v>
+        <f>(B196-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.3346248631777362</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
@@ -5765,8 +5765,8 @@
         <v>131939200</v>
       </c>
       <c r="H196">
-        <f>SPY_2[[#This Row],[Close]]-C195</f>
-        <v>-13.529998999999975</v>
+        <f>(B197-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>5.1056825749165459E-2</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
@@ -5792,8 +5792,8 @@
         <v>127637800</v>
       </c>
       <c r="H197">
-        <f>SPY_2[[#This Row],[Close]]-C196</f>
-        <v>-7.2700189999999907</v>
+        <f>(B198-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.3869739884605225</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
@@ -5819,8 +5819,8 @@
         <v>137167700</v>
       </c>
       <c r="H198">
-        <f>SPY_2[[#This Row],[Close]]-C197</f>
-        <v>-5.6499939999999924</v>
+        <f>(B199-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.59767807381717841</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
@@ -5846,8 +5846,8 @@
         <v>98977500</v>
       </c>
       <c r="H199">
-        <f>SPY_2[[#This Row],[Close]]-C198</f>
-        <v>-1.5099789999999871</v>
+        <f>(B200-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.2249601974222628</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
@@ -5873,8 +5873,8 @@
         <v>95484700</v>
       </c>
       <c r="H200">
-        <f>SPY_2[[#This Row],[Close]]-C199</f>
-        <v>7.4899899999999775</v>
+        <f>(B201-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>8.9692705410644696E-2</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
@@ -5900,8 +5900,8 @@
         <v>72238800</v>
       </c>
       <c r="H201">
-        <f>SPY_2[[#This Row],[Close]]-C200</f>
-        <v>0.63998400000002675</v>
+        <f>(B202-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.2917862992197372</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
@@ -5927,8 +5927,8 @@
         <v>61272600</v>
       </c>
       <c r="H202">
-        <f>SPY_2[[#This Row],[Close]]-C201</f>
-        <v>-3.6499939999999924</v>
+        <f>(B203-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.61756298122573261</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
@@ -5954,8 +5954,8 @@
         <v>76949400</v>
       </c>
       <c r="H203">
-        <f>SPY_2[[#This Row],[Close]]-C202</f>
-        <v>1.1099849999999947</v>
+        <f>(B204-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.11683477326835667</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
@@ -5981,8 +5981,8 @@
         <v>87724700</v>
       </c>
       <c r="H204">
-        <f>SPY_2[[#This Row],[Close]]-C203</f>
-        <v>-4.3299870000000169</v>
+        <f>(B205-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.74587113354673706</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
@@ -6008,8 +6008,8 @@
         <v>97264100</v>
       </c>
       <c r="H205">
-        <f>SPY_2[[#This Row],[Close]]-C204</f>
-        <v>-7.2000130000000127</v>
+        <f>(B206-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.2954938264681708E-2</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
@@ -6035,8 +6035,8 @@
         <v>116899300</v>
       </c>
       <c r="H206">
-        <f>SPY_2[[#This Row],[Close]]-C205</f>
-        <v>4.8600160000000301</v>
+        <f>(B207-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.4186147417941104</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
@@ -6062,8 +6062,8 @@
         <v>116568600</v>
       </c>
       <c r="H207">
-        <f>SPY_2[[#This Row],[Close]]-C206</f>
-        <v>-4.4099729999999795</v>
+        <f>(B208-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.0504928446652135</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
@@ -6089,8 +6089,8 @@
         <v>135511600</v>
       </c>
       <c r="H208">
-        <f>SPY_2[[#This Row],[Close]]-C207</f>
-        <v>-13</v>
+        <f>(B209-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.1720669012119451</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
@@ -6116,8 +6116,8 @@
         <v>107134800</v>
       </c>
       <c r="H209">
-        <f>SPY_2[[#This Row],[Close]]-C208</f>
-        <v>-9.7599789999999871</v>
+        <f>(B210-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.7978315337462164</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
@@ -6143,8 +6143,8 @@
         <v>69806300</v>
       </c>
       <c r="H210">
-        <f>SPY_2[[#This Row],[Close]]-C209</f>
-        <v>7.6600040000000149</v>
+        <f>(B211-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-5.8305403439320523E-2</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
@@ -6170,8 +6170,8 @@
         <v>58890200</v>
       </c>
       <c r="H211">
-        <f>SPY_2[[#This Row],[Close]]-C210</f>
-        <v>4.4800109999999904</v>
+        <f>(B212-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.22664542655756992</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.2">
@@ -6197,8 +6197,8 @@
         <v>56439700</v>
       </c>
       <c r="H212">
-        <f>SPY_2[[#This Row],[Close]]-C211</f>
-        <v>2.7900080000000003</v>
+        <f>(B213-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.31024054003093227</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
@@ -6224,8 +6224,8 @@
         <v>56808600</v>
       </c>
       <c r="H213">
-        <f>SPY_2[[#This Row],[Close]]-C212</f>
-        <v>5.0700080000000298</v>
+        <f>(B214-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>9.6381634824171045E-2</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
@@ -6251,8 +6251,8 @@
         <v>47274600</v>
       </c>
       <c r="H214">
-        <f>SPY_2[[#This Row],[Close]]-C213</f>
-        <v>-0.44000299999999015</v>
+        <f>(B215-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>2.3070438726171739E-2</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
@@ -6278,8 +6278,8 @@
         <v>54503000</v>
       </c>
       <c r="H215">
-        <f>SPY_2[[#This Row],[Close]]-C214</f>
-        <v>-1.3299870000000169</v>
+        <f>(B216-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>9.4241013159404086E-2</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
@@ -6305,8 +6305,8 @@
         <v>55329000</v>
       </c>
       <c r="H216">
-        <f>SPY_2[[#This Row],[Close]]-C215</f>
-        <v>-2.3999939999999924</v>
+        <f>(B217-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.10920467818208636</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
@@ -6332,8 +6332,8 @@
         <v>65237400</v>
       </c>
       <c r="H217">
-        <f>SPY_2[[#This Row],[Close]]-C216</f>
-        <v>-4.0400089999999977</v>
+        <f>(B218-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.28212839510517479</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
@@ -6359,8 +6359,8 @@
         <v>72668200</v>
       </c>
       <c r="H218">
-        <f>SPY_2[[#This Row],[Close]]-C217</f>
-        <v>0.85000600000000759</v>
+        <f>(B219-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.31609345176957426</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
@@ -6386,8 +6386,8 @@
         <v>71178700</v>
       </c>
       <c r="H219">
-        <f>SPY_2[[#This Row],[Close]]-C218</f>
-        <v>-0.30001800000002277</v>
+        <f>(B220-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-8.166349278600965E-2</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.2">
@@ -6413,8 +6413,8 @@
         <v>104538900</v>
       </c>
       <c r="H220">
-        <f>SPY_2[[#This Row],[Close]]-C219</f>
-        <v>-11.600006000000008</v>
+        <f>(B221-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.10461377402307716</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
@@ -6440,8 +6440,8 @@
         <v>86858900</v>
       </c>
       <c r="H221">
-        <f>SPY_2[[#This Row],[Close]]-C220</f>
-        <v>-10.040008999999998</v>
+        <f>(B222-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>2.1391631314354913E-3</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
@@ -6467,8 +6467,8 @@
         <v>85064800</v>
       </c>
       <c r="H222">
-        <f>SPY_2[[#This Row],[Close]]-C221</f>
-        <v>-4.7300109999999904</v>
+        <f>(B223-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.72732391364177018</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.2">
@@ -6494,8 +6494,8 @@
         <v>119362000</v>
       </c>
       <c r="H223">
-        <f>SPY_2[[#This Row],[Close]]-C222</f>
-        <v>-3.6900019999999927</v>
+        <f>(B224-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-6.0148867690306397E-2</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
@@ -6521,8 +6521,8 @@
         <v>74303100</v>
       </c>
       <c r="H224">
-        <f>SPY_2[[#This Row],[Close]]-C223</f>
-        <v>4.0100100000000225</v>
+        <f>(B225-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.39169686003192872</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.2">
@@ -6548,8 +6548,8 @@
         <v>67605400</v>
       </c>
       <c r="H225">
-        <f>SPY_2[[#This Row],[Close]]-C224</f>
-        <v>1.169983000000002</v>
+        <f>(B226-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.24839986143347795</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.2">
@@ -6575,8 +6575,8 @@
         <v>91173100</v>
       </c>
       <c r="H226">
-        <f>SPY_2[[#This Row],[Close]]-C225</f>
-        <v>-8.6700130000000399</v>
+        <f>(B227-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.71900566318430226</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.2">
@@ -6602,8 +6602,8 @@
         <v>95849600</v>
       </c>
       <c r="H227">
-        <f>SPY_2[[#This Row],[Close]]-C226</f>
-        <v>-8.1600039999999581</v>
+        <f>(B228-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.0716153789989442</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.2">
@@ -6629,8 +6629,8 @@
         <v>109709100</v>
       </c>
       <c r="H228">
-        <f>SPY_2[[#This Row],[Close]]-C227</f>
-        <v>-8.6000060000000076</v>
+        <f>(B229-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.35926636638845144</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.2">
@@ -6656,8 +6656,8 @@
         <v>109357600</v>
       </c>
       <c r="H229">
-        <f>SPY_2[[#This Row],[Close]]-C228</f>
-        <v>-8.2099910000000023</v>
+        <f>(B230-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.44272274488101826</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.2">
@@ -6683,8 +6683,8 @@
         <v>122379700</v>
       </c>
       <c r="H230">
-        <f>SPY_2[[#This Row],[Close]]-C229</f>
-        <v>-12.859984999999995</v>
+        <f>(B231-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.266368662562953</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.2">
@@ -6710,8 +6710,8 @@
         <v>202271200</v>
       </c>
       <c r="H231">
-        <f>SPY_2[[#This Row],[Close]]-C230</f>
-        <v>-20.759978999999987</v>
+        <f>(B232-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.3585122267143865</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
@@ -6737,8 +6737,8 @@
         <v>251783900</v>
       </c>
       <c r="H232">
-        <f>SPY_2[[#This Row],[Close]]-C231</f>
-        <v>-8.2200020000000222</v>
+        <f>(B233-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.5414691846259425</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.2">
@@ -6764,8 +6764,8 @@
         <v>167997300</v>
       </c>
       <c r="H233">
-        <f>SPY_2[[#This Row],[Close]]-C232</f>
-        <v>-5.9100039999999581</v>
+        <f>(B234-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.4385343028551238</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.2">
@@ -6791,8 +6791,8 @@
         <v>186391100</v>
       </c>
       <c r="H234">
-        <f>SPY_2[[#This Row],[Close]]-C233</f>
-        <v>-6.3399960000000419</v>
+        <f>(B235-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.1260337218372682</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.2">
@@ -6818,8 +6818,8 @@
         <v>149878300</v>
       </c>
       <c r="H235">
-        <f>SPY_2[[#This Row],[Close]]-C234</f>
-        <v>-12.80001900000002</v>
+        <f>(B236-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.33392148998056675</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.2">
@@ -6845,8 +6845,8 @@
         <v>164457400</v>
       </c>
       <c r="H236">
-        <f>SPY_2[[#This Row],[Close]]-C235</f>
-        <v>0.36001600000003009</v>
+        <f>(B237-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.16065663100378819</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.2">
@@ -6872,8 +6872,8 @@
         <v>152251400</v>
       </c>
       <c r="H237">
-        <f>SPY_2[[#This Row],[Close]]-C236</f>
-        <v>7.9100040000000149</v>
+        <f>(B238-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.17114289372414346</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.2">
@@ -6899,8 +6899,8 @@
         <v>123155400</v>
       </c>
       <c r="H238">
-        <f>SPY_2[[#This Row],[Close]]-C237</f>
-        <v>2.6700130000000399</v>
+        <f>(B239-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.56297338170729194</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.2">
@@ -6926,8 +6926,8 @@
         <v>117361000</v>
       </c>
       <c r="H239">
-        <f>SPY_2[[#This Row],[Close]]-C238</f>
-        <v>3.7200010000000248</v>
+        <f>(B240-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.3993645820570935</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.2">
@@ -6953,8 +6953,8 @@
         <v>118024400</v>
       </c>
       <c r="H240">
-        <f>SPY_2[[#This Row],[Close]]-C239</f>
-        <v>-11.51998900000001</v>
+        <f>(B241-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-5.5978503502304031E-2</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.2">
@@ -6980,8 +6980,8 @@
         <v>118335600</v>
       </c>
       <c r="H241">
-        <f>SPY_2[[#This Row],[Close]]-C240</f>
-        <v>-4.2699890000000096</v>
+        <f>(B242-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.1805210560145934</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
@@ -7007,8 +7007,8 @@
         <v>84472900</v>
       </c>
       <c r="H242">
-        <f>SPY_2[[#This Row],[Close]]-C241</f>
-        <v>-5.5199889999999527</v>
+        <f>(B243-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.11849908065781067</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
@@ -7034,8 +7034,8 @@
         <v>81012000</v>
       </c>
       <c r="H243">
-        <f>SPY_2[[#This Row],[Close]]-C242</f>
-        <v>-4.9987999999984822E-2</v>
+        <f>(B244-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.94912826119161464</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.2">
@@ -7061,8 +7061,8 @@
         <v>92589900</v>
       </c>
       <c r="H244">
-        <f>SPY_2[[#This Row],[Close]]-C243</f>
-        <v>5.6199960000000146</v>
+        <f>(B245-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-1.3550755951486666</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.2">
@@ -7088,8 +7088,8 @@
         <v>140103700</v>
       </c>
       <c r="H245">
-        <f>SPY_2[[#This Row],[Close]]-C244</f>
-        <v>-8.5599980000000073</v>
+        <f>(B246-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>2.0029599972840605E-2</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.2">
@@ -7115,8 +7115,8 @@
         <v>153064100</v>
       </c>
       <c r="H246">
-        <f>SPY_2[[#This Row],[Close]]-C245</f>
-        <v>-17.25</v>
+        <f>(B247-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.12259410866673227</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.2">
@@ -7142,8 +7142,8 @@
         <v>123006300</v>
       </c>
       <c r="H247">
-        <f>SPY_2[[#This Row],[Close]]-C246</f>
-        <v>-12.589995999999985</v>
+        <f>(B248-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>1.0728490998162685</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.2">
@@ -7169,8 +7169,8 @@
         <v>88659500</v>
       </c>
       <c r="H248">
-        <f>SPY_2[[#This Row],[Close]]-C247</f>
-        <v>4.5</v>
+        <f>(B249-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.48644092598375421</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.2">
@@ -7196,8 +7196,8 @@
         <v>84863600</v>
       </c>
       <c r="H249">
-        <f>SPY_2[[#This Row],[Close]]-C248</f>
-        <v>0.32000700000003235</v>
+        <f>(B250-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.75683048692121668</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.2">
@@ -7223,8 +7223,8 @@
         <v>102259100</v>
       </c>
       <c r="H250">
-        <f>SPY_2[[#This Row],[Close]]-C249</f>
-        <v>-11</v>
+        <f>(B251-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>6.1773898603278164E-2</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.2">
@@ -7250,8 +7250,8 @@
         <v>132454300</v>
       </c>
       <c r="H251">
-        <f>SPY_2[[#This Row],[Close]]-C250</f>
-        <v>-12.339995999999985</v>
+        <f>(B252-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-0.53888398791487147</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.2">
@@ -7277,8 +7277,8 @@
         <v>124391800</v>
       </c>
       <c r="H252">
-        <f>SPY_2[[#This Row],[Close]]-C251</f>
-        <v>-9.0899970000000394</v>
+        <f>(B253-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>0.71932326504351118</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.2">
@@ -7304,8 +7304,8 @@
         <v>132578000</v>
       </c>
       <c r="H253">
-        <f>SPY_2[[#This Row],[Close]]-C252</f>
-        <v>-13.549987999999985</v>
+        <f>(B254-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-2.5903596845969528</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.2">
@@ -7331,8 +7331,8 @@
         <v>213570500</v>
       </c>
       <c r="H254">
-        <f>SPY_2[[#This Row],[Close]]-C253</f>
-        <v>-4.9600220000000377</v>
+        <f>(B255-SPY_2[[#This Row],[Close]]) / SPY_2[[#This Row],[Close]] * 100</f>
+        <v>-100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>